<commit_message>
A finished the initial state
</commit_message>
<xml_diff>
--- a/app/config/tables/MADTRIAL_FU_PHONE/Forms/MADTRIAL_FU_PHONE/MADTRIAL_FU_PHONE.xlsx
+++ b/app/config/tables/MADTRIAL_FU_PHONE/Forms/MADTRIAL_FU_PHONE/MADTRIAL_FU_PHONE.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="143">
   <si>
     <t>setting_name</t>
   </si>
@@ -164,16 +164,301 @@
     <t>DATSEGUI</t>
   </si>
   <si>
-    <t>Type</t>
-  </si>
-  <si>
     <t>Data da ligação</t>
   </si>
   <si>
-    <t>Integre</t>
-  </si>
-  <si>
     <t>TELENUM1</t>
+  </si>
+  <si>
+    <t>Assistente</t>
+  </si>
+  <si>
+    <t>ASSISTENTE</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>Numero de telemovel</t>
+  </si>
+  <si>
+    <t>select_one</t>
+  </si>
+  <si>
+    <t>cham</t>
+  </si>
+  <si>
+    <t>CHAMADA1</t>
+  </si>
+  <si>
+    <t>1 a Chamada</t>
+  </si>
+  <si>
+    <t>Seguimento realizado</t>
+  </si>
+  <si>
+    <t>Sem rede</t>
+  </si>
+  <si>
+    <t>não atende o telemovel</t>
+  </si>
+  <si>
+    <t>Numero Incorreto</t>
+  </si>
+  <si>
+    <t>Se voce não conseguir obter informação na primeira chamada, tente cada numero trez vezes</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>TELENUM2</t>
+  </si>
+  <si>
+    <t>CHAMADA2</t>
+  </si>
+  <si>
+    <t>2 a Chamada</t>
+  </si>
+  <si>
+    <t>TELENUM3</t>
+  </si>
+  <si>
+    <t>3 a Chamada</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>INFORMADOR</t>
+  </si>
+  <si>
+    <t>Informador</t>
+  </si>
+  <si>
+    <t>Mae</t>
+  </si>
+  <si>
+    <t>Outro</t>
+  </si>
+  <si>
+    <t>Outro zelador</t>
+  </si>
+  <si>
+    <t>Ninguem para fornecer informaçeos</t>
+  </si>
+  <si>
+    <t>sim/não</t>
+  </si>
+  <si>
+    <t>VITALCRI</t>
+  </si>
+  <si>
+    <t>sim</t>
+  </si>
+  <si>
+    <t>não</t>
+  </si>
+  <si>
+    <t>sim/não/nãosabe</t>
+  </si>
+  <si>
+    <t>não sabe</t>
+  </si>
+  <si>
+    <t>DOD</t>
+  </si>
+  <si>
+    <t>Data do felecimento</t>
+  </si>
+  <si>
+    <t>VACHIS</t>
+  </si>
+  <si>
+    <t>A criança recebeu outras vacinas desde que foi vacinada no Simão Mendes?</t>
+  </si>
+  <si>
+    <t>select_multiple</t>
+  </si>
+  <si>
+    <t>vac</t>
+  </si>
+  <si>
+    <t>VACTIPO</t>
+  </si>
+  <si>
+    <t>Qual vacinas?</t>
+  </si>
+  <si>
+    <t>BCG</t>
+  </si>
+  <si>
+    <t>VPO</t>
+  </si>
+  <si>
+    <t>Penta</t>
+  </si>
+  <si>
+    <t>PCV</t>
+  </si>
+  <si>
+    <t>Rota</t>
+  </si>
+  <si>
+    <t>Sarampo</t>
+  </si>
+  <si>
+    <t>Febre Amarelo</t>
+  </si>
+  <si>
+    <t>VACOUTRO</t>
+  </si>
+  <si>
+    <t>Outro Vacina</t>
+  </si>
+  <si>
+    <t>HOSPI</t>
+  </si>
+  <si>
+    <t>A criança foi internada no hospital desde que foi vacinada contra sarampo em Simão Mendes?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adate </t>
+  </si>
+  <si>
+    <t>HOSPDATA1</t>
+  </si>
+  <si>
+    <t>Data do Primeiro Internamento</t>
+  </si>
+  <si>
+    <t>if</t>
+  </si>
+  <si>
+    <t>end if</t>
+  </si>
+  <si>
+    <t>data('HOSPI')=="1"</t>
+  </si>
+  <si>
+    <t>HOSPCODE1</t>
+  </si>
+  <si>
+    <t>Local do primeiro Internamento</t>
+  </si>
+  <si>
+    <t>HOSPCAUSA1</t>
+  </si>
+  <si>
+    <t>Causa do primeiro Internamento</t>
+  </si>
+  <si>
+    <t>HOSPDIAS1</t>
+  </si>
+  <si>
+    <t>Duração do primeiro Internamento  em dias</t>
+  </si>
+  <si>
+    <t>HOSPI2</t>
+  </si>
+  <si>
+    <t>A criança foi enternada no hospital mais de um vez?</t>
+  </si>
+  <si>
+    <t>HOSPDATA2</t>
+  </si>
+  <si>
+    <t>Local do segundo Internamento</t>
+  </si>
+  <si>
+    <t>HOSPCAUSA2</t>
+  </si>
+  <si>
+    <t>Data do segundo Internamento</t>
+  </si>
+  <si>
+    <t>HOSPDIA2</t>
+  </si>
+  <si>
+    <t>Duração do segundo Internamento</t>
+  </si>
+  <si>
+    <t>HOSPALTA2</t>
+  </si>
+  <si>
+    <t>A criança esta ainda Internada</t>
+  </si>
+  <si>
+    <t>HOSPCODE2</t>
+  </si>
+  <si>
+    <t>Causa de segundo Internamento</t>
+  </si>
+  <si>
+    <t>HOSPALTA</t>
+  </si>
+  <si>
+    <t>A criança esta ainda internada</t>
+  </si>
+  <si>
+    <t>data('HOSPI2')=="1"</t>
+  </si>
+  <si>
+    <t>HOSPI3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if </t>
+  </si>
+  <si>
+    <t>data('HOSPI3')=="1"</t>
+  </si>
+  <si>
+    <t>HOSPDATA3</t>
+  </si>
+  <si>
+    <t>Data do terceiro Internamento</t>
+  </si>
+  <si>
+    <t>Local do terceiro Internamento</t>
+  </si>
+  <si>
+    <t>Causa do terceiro Internamento</t>
+  </si>
+  <si>
+    <t>Duraçao do terceiro Internamento em dias</t>
+  </si>
+  <si>
+    <t>HOSPCODE3</t>
+  </si>
+  <si>
+    <t>HOSPCAUSA3</t>
+  </si>
+  <si>
+    <t>HOSPDIAS3</t>
+  </si>
+  <si>
+    <t>HOSPALTA3</t>
+  </si>
+  <si>
+    <t>a criança esta ainda Internada</t>
+  </si>
+  <si>
+    <t>PODEAUT</t>
+  </si>
+  <si>
+    <t>Podemos visita-lo para fazer mais perguntas sobre a morte de seu filho</t>
+  </si>
+  <si>
+    <t>A criança ainda esta viva?</t>
+  </si>
+  <si>
+    <t>A criança foi Internada no hospital mais de duas vezes?</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>data('VITALCRI')=="2"</t>
   </si>
 </sst>
 </file>
@@ -687,11 +972,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="94" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -743,13 +1028,13 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D3" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
         <v>43</v>
       </c>
       <c r="H3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -764,37 +1049,627 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F6" t="s">
         <v>47</v>
       </c>
+      <c r="H6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="D9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
       <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E12" s="4"/>
+      <c r="D12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" t="s">
+        <v>52</v>
+      </c>
+      <c r="H12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="D15" t="s">
+        <v>141</v>
+      </c>
+      <c r="H15" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
       <c r="G16" s="14"/>
     </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D18" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" t="s">
+        <v>60</v>
+      </c>
+      <c r="H18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D21" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" t="s">
+        <v>61</v>
+      </c>
+      <c r="H21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C24" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="46" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="D24" t="s">
+        <v>59</v>
+      </c>
+      <c r="F24" t="s">
+        <v>63</v>
+      </c>
+      <c r="H24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D27" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" t="s">
+        <v>65</v>
+      </c>
+      <c r="F27" t="s">
+        <v>66</v>
+      </c>
+      <c r="H27" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D30" t="s">
+        <v>50</v>
+      </c>
+      <c r="E30" t="s">
+        <v>76</v>
+      </c>
+      <c r="F30" t="s">
+        <v>73</v>
+      </c>
+      <c r="H30" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
+        <v>100</v>
+      </c>
+      <c r="C31" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D32" t="s">
+        <v>30</v>
+      </c>
+      <c r="F32" t="s">
+        <v>78</v>
+      </c>
+      <c r="H32" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B33" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D36" t="s">
+        <v>50</v>
+      </c>
+      <c r="E36" t="s">
+        <v>76</v>
+      </c>
+      <c r="F36" t="s">
+        <v>80</v>
+      </c>
+      <c r="H36" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B38" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D39" t="s">
+        <v>82</v>
+      </c>
+      <c r="E39" t="s">
+        <v>83</v>
+      </c>
+      <c r="F39" t="s">
+        <v>84</v>
+      </c>
+      <c r="H39" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B41" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D42" t="s">
+        <v>48</v>
+      </c>
+      <c r="F42" t="s">
+        <v>93</v>
+      </c>
+      <c r="H42" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B43" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B44" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D45" t="s">
+        <v>50</v>
+      </c>
+      <c r="E45" t="s">
+        <v>76</v>
+      </c>
+      <c r="F45" t="s">
+        <v>95</v>
+      </c>
+      <c r="H45" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B46" t="s">
+        <v>41</v>
+      </c>
       <c r="H46" s="4"/>
     </row>
-    <row r="47" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H47" s="4"/>
-    </row>
-    <row r="48" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B47" t="s">
+        <v>100</v>
+      </c>
+      <c r="C47" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B48" t="s">
+        <v>40</v>
+      </c>
       <c r="H48" s="4"/>
     </row>
-    <row r="49" spans="8:8" x14ac:dyDescent="0.35">
-      <c r="H49" s="4"/>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D49" t="s">
+        <v>97</v>
+      </c>
+      <c r="F49" t="s">
+        <v>98</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D50" t="s">
+        <v>48</v>
+      </c>
+      <c r="F50" t="s">
+        <v>103</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D51" t="s">
+        <v>48</v>
+      </c>
+      <c r="F51" t="s">
+        <v>105</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D52" t="s">
+        <v>59</v>
+      </c>
+      <c r="F52" t="s">
+        <v>107</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D53" t="s">
+        <v>48</v>
+      </c>
+      <c r="F53" t="s">
+        <v>121</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B54" t="s">
+        <v>41</v>
+      </c>
+      <c r="H54" s="4"/>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B55" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D56" t="s">
+        <v>50</v>
+      </c>
+      <c r="E56" t="s">
+        <v>76</v>
+      </c>
+      <c r="F56" t="s">
+        <v>109</v>
+      </c>
+      <c r="H56" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B57" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B58" t="s">
+        <v>100</v>
+      </c>
+      <c r="C58" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B59" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D60" t="s">
+        <v>30</v>
+      </c>
+      <c r="F60" t="s">
+        <v>111</v>
+      </c>
+      <c r="H60" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D61" t="s">
+        <v>48</v>
+      </c>
+      <c r="F61" t="s">
+        <v>113</v>
+      </c>
+      <c r="H61" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D62" t="s">
+        <v>48</v>
+      </c>
+      <c r="F62" t="s">
+        <v>119</v>
+      </c>
+      <c r="H62" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D63" t="s">
+        <v>59</v>
+      </c>
+      <c r="F63" t="s">
+        <v>115</v>
+      </c>
+      <c r="H63" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D64" t="s">
+        <v>48</v>
+      </c>
+      <c r="F64" t="s">
+        <v>117</v>
+      </c>
+      <c r="H64" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B65" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B66" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D67" t="s">
+        <v>50</v>
+      </c>
+      <c r="E67" t="s">
+        <v>76</v>
+      </c>
+      <c r="F67" t="s">
+        <v>124</v>
+      </c>
+      <c r="H67" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B68" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B69" t="s">
+        <v>125</v>
+      </c>
+      <c r="C69" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B70" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D71" t="s">
+        <v>30</v>
+      </c>
+      <c r="F71" t="s">
+        <v>127</v>
+      </c>
+      <c r="H71" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D72" t="s">
+        <v>48</v>
+      </c>
+      <c r="F72" t="s">
+        <v>132</v>
+      </c>
+      <c r="H72" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D73" t="s">
+        <v>48</v>
+      </c>
+      <c r="F73" t="s">
+        <v>133</v>
+      </c>
+      <c r="H73" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D74" t="s">
+        <v>59</v>
+      </c>
+      <c r="F74" t="s">
+        <v>134</v>
+      </c>
+      <c r="H74" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D75" t="s">
+        <v>48</v>
+      </c>
+      <c r="F75" t="s">
+        <v>135</v>
+      </c>
+      <c r="H75" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B76" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B77" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B78" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B79" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B80" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="D81" t="s">
+        <v>50</v>
+      </c>
+      <c r="E81" t="s">
+        <v>72</v>
+      </c>
+      <c r="F81" t="s">
+        <v>137</v>
+      </c>
+      <c r="H81" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B82" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -808,7 +1683,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:D20"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -833,64 +1708,261 @@
         <v>14</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="str">
+        <f>"1"</f>
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>54</v>
+      </c>
+    </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B3" s="2"/>
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="2" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D4" s="2"/>
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="str">
+        <f>"3"</f>
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D5" s="2"/>
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="str">
+        <f>"4"</f>
+        <v>4</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D6" s="2"/>
+      <c r="A6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" t="str">
+        <f>"1"</f>
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D7" s="2"/>
+      <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" t="str">
+        <f>"3"</f>
+        <v>3</v>
+      </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" t="str">
+        <f>"4"</f>
+        <v>4</v>
+      </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" t="str">
+        <f>"1"</f>
+        <v>1</v>
+      </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D11" s="2"/>
+      <c r="A11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D12" s="2"/>
+      <c r="A12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" t="str">
+        <f>"3"</f>
+        <v>3</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D13" s="2"/>
+      <c r="A13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" t="str">
+        <f>"1"</f>
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D14" s="2"/>
+      <c r="A14" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D15" s="2"/>
+      <c r="A15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" t="str">
+        <f>"3"</f>
+        <v>3</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D20" s="2"/>
+      <c r="A16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" t="str">
+        <f>"4"</f>
+        <v>4</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" t="str">
+        <f>"5"</f>
+        <v>5</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" t="str">
+        <f>"6"</f>
+        <v>6</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" t="str">
+        <f>"7"</f>
+        <v>7</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>83</v>
+      </c>
+      <c r="B20" t="str">
+        <f>"8"</f>
+        <v>8</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" t="str">
+        <f>"1"</f>
+        <v>1</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" s="4"/>

</xml_diff>